<commit_message>
significant remote updates during shutdown
</commit_message>
<xml_diff>
--- a/analysis/data/NCRMP_Pacific_AllBMUdata.xlsx
+++ b/analysis/data/NCRMP_Pacific_AllBMUdata.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ienoc\Documents\GitHub\globalBar\analysis\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F6D7F34-CDE2-43DF-AFD9-BC13E0983C28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E7453A80-8B4C-4F32-94CA-F14AC1207990}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="19110" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="12320" yWindow="2690" windowWidth="26080" windowHeight="15770" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5553" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5005" uniqueCount="171">
   <si>
     <t>region</t>
   </si>
@@ -877,8 +877,8 @@
   <dimension ref="A1:AM1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E253" sqref="E253:F253"/>
+      <pane ySplit="1" topLeftCell="A980" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A1000" sqref="A453:XFD1000"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.25" defaultRowHeight="15" customHeight="1"/>
@@ -41157,2746 +41157,554 @@
       </c>
       <c r="AM452" s="2"/>
     </row>
-    <row r="453" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A453" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="454" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A454" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="455" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A455" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="456" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A456" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="457" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A457" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="458" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A458" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="459" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A459" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="460" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A460" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="461" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A461" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="462" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A462" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="463" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A463" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="464" spans="1:39" ht="15.75" customHeight="1">
-      <c r="A464" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="465" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A465" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="466" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A466" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="467" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A467" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="468" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A468" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="469" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A469" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="470" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A470" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="471" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A471" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="472" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A472" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="473" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A473" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="474" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A474" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="475" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A475" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="476" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A476" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="477" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A477" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="478" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A478" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="479" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A479" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="480" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A480" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="481" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A481" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="482" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A482" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="483" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A483" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="484" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A484" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="485" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A485" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="486" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A486" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="487" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A487" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="488" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A488" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="489" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A489" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="490" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A490" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="491" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A491" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="492" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A492" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="493" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A493" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="494" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A494" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="495" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A495" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="496" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A496" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="497" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A497" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="498" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A498" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="499" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A499" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="500" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A500" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="501" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A501" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="502" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A502" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="503" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A503" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="504" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A504" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="505" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A505" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="506" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A506" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="507" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A507" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="508" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A508" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="509" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A509" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="510" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A510" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="511" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A511" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="512" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A512" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="513" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A513" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="514" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A514" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="515" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A515" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="516" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A516" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="517" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A517" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="518" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A518" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="519" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A519" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="520" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A520" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="521" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A521" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="522" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A522" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="523" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A523" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="524" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A524" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="525" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A525" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="526" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A526" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="527" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A527" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="528" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A528" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="529" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A529" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="530" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A530" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="531" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A531" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="532" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A532" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="533" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A533" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="534" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A534" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="535" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A535" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="536" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A536" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="537" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A537" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="538" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A538" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="539" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A539" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="540" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A540" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="541" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A541" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="542" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A542" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="543" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A543" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="544" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A544" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="545" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A545" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="546" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A546" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="547" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A547" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="548" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A548" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="549" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A549" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="550" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A550" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="551" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A551" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="552" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A552" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="553" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A553" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="554" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A554" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="555" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A555" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="556" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A556" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="557" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A557" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="558" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A558" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="559" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A559" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="560" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A560" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="561" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A561" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="562" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A562" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="563" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A563" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="564" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A564" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="565" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A565" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="566" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A566" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="567" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A567" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="568" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A568" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="569" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A569" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="570" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A570" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="571" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A571" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="572" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A572" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="573" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A573" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="574" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A574" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="575" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A575" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="576" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A576" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="577" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A577" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="578" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A578" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="579" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A579" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="580" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A580" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="581" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A581" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="582" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A582" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="583" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A583" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="584" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A584" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="585" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A585" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="586" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A586" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="587" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A587" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="588" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A588" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="589" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A589" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="590" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A590" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="591" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A591" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="592" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A592" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="593" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A593" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="594" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A594" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="595" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A595" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="596" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A596" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="597" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A597" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="598" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A598" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="599" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A599" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="600" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A600" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="601" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A601" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="602" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A602" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="603" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A603" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="604" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A604" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="605" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A605" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="606" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A606" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="607" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A607" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="608" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A608" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="609" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A609" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="610" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A610" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="611" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A611" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="612" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A612" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="613" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A613" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="614" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A614" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="615" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A615" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="616" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A616" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="617" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A617" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="618" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A618" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="619" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A619" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="620" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A620" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="621" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A621" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="622" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A622" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="623" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A623" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="624" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A624" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="625" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A625" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="626" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A626" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="627" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A627" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="628" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A628" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="629" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A629" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="630" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A630" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="631" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A631" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="632" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A632" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="633" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A633" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="634" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A634" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="635" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A635" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="636" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A636" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="637" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A637" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="638" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A638" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="639" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A639" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="640" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A640" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="641" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A641" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="642" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A642" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="643" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A643" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="644" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A644" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="645" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A645" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="646" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A646" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="647" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A647" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="648" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A648" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="649" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A649" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="650" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A650" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="651" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A651" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="652" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A652" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="653" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A653" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="654" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A654" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="655" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A655" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="656" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A656" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="657" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A657" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="658" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A658" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="659" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A659" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="660" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A660" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="661" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A661" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="662" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A662" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="663" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A663" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="664" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A664" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="665" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A665" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="666" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A666" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="667" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A667" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="668" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A668" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="669" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A669" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="670" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A670" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="671" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A671" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="672" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A672" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="673" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A673" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="674" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A674" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="675" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A675" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="676" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A676" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="677" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A677" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="678" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A678" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="679" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A679" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="680" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A680" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="681" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A681" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="682" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A682" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="683" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A683" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="684" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A684" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="685" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A685" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="686" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A686" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="687" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A687" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="688" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A688" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="689" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A689" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="690" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A690" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="691" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A691" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="692" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A692" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="693" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A693" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="694" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A694" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="695" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A695" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="696" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A696" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="697" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A697" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="698" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A698" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="699" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A699" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="700" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A700" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="701" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A701" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="702" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A702" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="703" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A703" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="704" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A704" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="705" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A705" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="706" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A706" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="707" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A707" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="708" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A708" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="709" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A709" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="710" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A710" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="711" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A711" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="712" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A712" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="713" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A713" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="714" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A714" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="715" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A715" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="716" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A716" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="717" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A717" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="718" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A718" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="719" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A719" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="720" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A720" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="721" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A721" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="722" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A722" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="723" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A723" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="724" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A724" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="725" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A725" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="726" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A726" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="727" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A727" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="728" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A728" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="729" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A729" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="730" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A730" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="731" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A731" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="732" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A732" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="733" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A733" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="734" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A734" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="735" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A735" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="736" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A736" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="737" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A737" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="738" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A738" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="739" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A739" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="740" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A740" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="741" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A741" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="742" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A742" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="743" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A743" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="744" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A744" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="745" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A745" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="746" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A746" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="747" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A747" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="748" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A748" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="749" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A749" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="750" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A750" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="751" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A751" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="752" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A752" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="753" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A753" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="754" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A754" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="755" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A755" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="756" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A756" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="757" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A757" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="758" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A758" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="759" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A759" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="760" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A760" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="761" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A761" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="762" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A762" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="763" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A763" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="764" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A764" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="765" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A765" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="766" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A766" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="767" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A767" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="768" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A768" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="769" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A769" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="770" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A770" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="771" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A771" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="772" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A772" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="773" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A773" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="774" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A774" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="775" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A775" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="776" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A776" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="777" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A777" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="778" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A778" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="779" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A779" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="780" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A780" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="781" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A781" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="782" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A782" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="783" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A783" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="784" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A784" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="785" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A785" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="786" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A786" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="787" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A787" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="788" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A788" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="789" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A789" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="790" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A790" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="791" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A791" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="792" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A792" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="793" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A793" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="794" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A794" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="795" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A795" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="796" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A796" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="797" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A797" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="798" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A798" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="799" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A799" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="800" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A800" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="801" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A801" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="802" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A802" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="803" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A803" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="804" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A804" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="805" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A805" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="806" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A806" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="807" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A807" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="808" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A808" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="809" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A809" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="810" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A810" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="811" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A811" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="812" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A812" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="813" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A813" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="814" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A814" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="815" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A815" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="816" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A816" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="817" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A817" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="818" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A818" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="819" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A819" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="820" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A820" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="821" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A821" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="822" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A822" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="823" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A823" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="824" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A824" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="825" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A825" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="826" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A826" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="827" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A827" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="828" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A828" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="829" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A829" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="830" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A830" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="831" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A831" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="832" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A832" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="833" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A833" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="834" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A834" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="835" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A835" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="836" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A836" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="837" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A837" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="838" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A838" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="839" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A839" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="840" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A840" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="841" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A841" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="842" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A842" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="843" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A843" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="844" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A844" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="845" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A845" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="846" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A846" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="847" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A847" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="848" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A848" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="849" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A849" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="850" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A850" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="851" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A851" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="852" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A852" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="853" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A853" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="854" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A854" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="855" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A855" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="856" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A856" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="857" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A857" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="858" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A858" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="859" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A859" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="860" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A860" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="861" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A861" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="862" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A862" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="863" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A863" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="864" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A864" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="865" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A865" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="866" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A866" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="867" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A867" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="868" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A868" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="869" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A869" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="870" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A870" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="871" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A871" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="872" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A872" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="873" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A873" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="874" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A874" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="875" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A875" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="876" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A876" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="877" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A877" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="878" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A878" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="879" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A879" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="880" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A880" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="881" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A881" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="882" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A882" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="883" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A883" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="884" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A884" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="885" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A885" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="886" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A886" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="887" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A887" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="888" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A888" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="889" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A889" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="890" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A890" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="891" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A891" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="892" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A892" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="893" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A893" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="894" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A894" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="895" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A895" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="896" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A896" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="897" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A897" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="898" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A898" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="899" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A899" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="900" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A900" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="901" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A901" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="902" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A902" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="903" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A903" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="904" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A904" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="905" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A905" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="906" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A906" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="907" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A907" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="908" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A908" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="909" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A909" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="910" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A910" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="911" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A911" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="912" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A912" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="913" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A913" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="914" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A914" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="915" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A915" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="916" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A916" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="917" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A917" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="918" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A918" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="919" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A919" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="920" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A920" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="921" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A921" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="922" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A922" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="923" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A923" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="924" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A924" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="925" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A925" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="926" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A926" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="927" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A927" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="928" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A928" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="929" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A929" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="930" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A930" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="931" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A931" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="932" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A932" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="933" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A933" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="934" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A934" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="935" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A935" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="936" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A936" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="937" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A937" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="938" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A938" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="939" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A939" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="940" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A940" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="941" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A941" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="942" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A942" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="943" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A943" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="944" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A944" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="945" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A945" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="946" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A946" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="947" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A947" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="948" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A948" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="949" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A949" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="950" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A950" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="951" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A951" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="952" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A952" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="953" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A953" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="954" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A954" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="955" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A955" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="956" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A956" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="957" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A957" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="958" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A958" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="959" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A959" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="960" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A960" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="961" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A961" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="962" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A962" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="963" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A963" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="964" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A964" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="965" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A965" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="966" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A966" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="967" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A967" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="968" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A968" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="969" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A969" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="970" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A970" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="971" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A971" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="972" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A972" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="973" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A973" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="974" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A974" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="975" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A975" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="976" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A976" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="977" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A977" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="978" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A978" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="979" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A979" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="980" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A980" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="981" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A981" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="982" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A982" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="983" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A983" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="984" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A984" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="985" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A985" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="986" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A986" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="987" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A987" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="988" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A988" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="989" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A989" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="990" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A990" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="991" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A991" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="992" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A992" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="993" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A993" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="994" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A994" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="995" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A995" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="996" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A996" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="997" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A997" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="998" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A998" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="999" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A999" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="1000" spans="1:1" ht="15.75" customHeight="1">
-      <c r="A1000" t="s">
-        <v>167</v>
-      </c>
-    </row>
+    <row r="453" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="454" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="455" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="456" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="457" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="458" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="459" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="460" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="461" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="462" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="463" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="464" spans="1:39" ht="15.75" customHeight="1"/>
+    <row r="465" ht="15.75" customHeight="1"/>
+    <row r="466" ht="15.75" customHeight="1"/>
+    <row r="467" ht="15.75" customHeight="1"/>
+    <row r="468" ht="15.75" customHeight="1"/>
+    <row r="469" ht="15.75" customHeight="1"/>
+    <row r="470" ht="15.75" customHeight="1"/>
+    <row r="471" ht="15.75" customHeight="1"/>
+    <row r="472" ht="15.75" customHeight="1"/>
+    <row r="473" ht="15.75" customHeight="1"/>
+    <row r="474" ht="15.75" customHeight="1"/>
+    <row r="475" ht="15.75" customHeight="1"/>
+    <row r="476" ht="15.75" customHeight="1"/>
+    <row r="477" ht="15.75" customHeight="1"/>
+    <row r="478" ht="15.75" customHeight="1"/>
+    <row r="479" ht="15.75" customHeight="1"/>
+    <row r="480" ht="15.75" customHeight="1"/>
+    <row r="481" ht="15.75" customHeight="1"/>
+    <row r="482" ht="15.75" customHeight="1"/>
+    <row r="483" ht="15.75" customHeight="1"/>
+    <row r="484" ht="15.75" customHeight="1"/>
+    <row r="485" ht="15.75" customHeight="1"/>
+    <row r="486" ht="15.75" customHeight="1"/>
+    <row r="487" ht="15.75" customHeight="1"/>
+    <row r="488" ht="15.75" customHeight="1"/>
+    <row r="489" ht="15.75" customHeight="1"/>
+    <row r="490" ht="15.75" customHeight="1"/>
+    <row r="491" ht="15.75" customHeight="1"/>
+    <row r="492" ht="15.75" customHeight="1"/>
+    <row r="493" ht="15.75" customHeight="1"/>
+    <row r="494" ht="15.75" customHeight="1"/>
+    <row r="495" ht="15.75" customHeight="1"/>
+    <row r="496" ht="15.75" customHeight="1"/>
+    <row r="497" ht="15.75" customHeight="1"/>
+    <row r="498" ht="15.75" customHeight="1"/>
+    <row r="499" ht="15.75" customHeight="1"/>
+    <row r="500" ht="15.75" customHeight="1"/>
+    <row r="501" ht="15.75" customHeight="1"/>
+    <row r="502" ht="15.75" customHeight="1"/>
+    <row r="503" ht="15.75" customHeight="1"/>
+    <row r="504" ht="15.75" customHeight="1"/>
+    <row r="505" ht="15.75" customHeight="1"/>
+    <row r="506" ht="15.75" customHeight="1"/>
+    <row r="507" ht="15.75" customHeight="1"/>
+    <row r="508" ht="15.75" customHeight="1"/>
+    <row r="509" ht="15.75" customHeight="1"/>
+    <row r="510" ht="15.75" customHeight="1"/>
+    <row r="511" ht="15.75" customHeight="1"/>
+    <row r="512" ht="15.75" customHeight="1"/>
+    <row r="513" ht="15.75" customHeight="1"/>
+    <row r="514" ht="15.75" customHeight="1"/>
+    <row r="515" ht="15.75" customHeight="1"/>
+    <row r="516" ht="15.75" customHeight="1"/>
+    <row r="517" ht="15.75" customHeight="1"/>
+    <row r="518" ht="15.75" customHeight="1"/>
+    <row r="519" ht="15.75" customHeight="1"/>
+    <row r="520" ht="15.75" customHeight="1"/>
+    <row r="521" ht="15.75" customHeight="1"/>
+    <row r="522" ht="15.75" customHeight="1"/>
+    <row r="523" ht="15.75" customHeight="1"/>
+    <row r="524" ht="15.75" customHeight="1"/>
+    <row r="525" ht="15.75" customHeight="1"/>
+    <row r="526" ht="15.75" customHeight="1"/>
+    <row r="527" ht="15.75" customHeight="1"/>
+    <row r="528" ht="15.75" customHeight="1"/>
+    <row r="529" ht="15.75" customHeight="1"/>
+    <row r="530" ht="15.75" customHeight="1"/>
+    <row r="531" ht="15.75" customHeight="1"/>
+    <row r="532" ht="15.75" customHeight="1"/>
+    <row r="533" ht="15.75" customHeight="1"/>
+    <row r="534" ht="15.75" customHeight="1"/>
+    <row r="535" ht="15.75" customHeight="1"/>
+    <row r="536" ht="15.75" customHeight="1"/>
+    <row r="537" ht="15.75" customHeight="1"/>
+    <row r="538" ht="15.75" customHeight="1"/>
+    <row r="539" ht="15.75" customHeight="1"/>
+    <row r="540" ht="15.75" customHeight="1"/>
+    <row r="541" ht="15.75" customHeight="1"/>
+    <row r="542" ht="15.75" customHeight="1"/>
+    <row r="543" ht="15.75" customHeight="1"/>
+    <row r="544" ht="15.75" customHeight="1"/>
+    <row r="545" ht="15.75" customHeight="1"/>
+    <row r="546" ht="15.75" customHeight="1"/>
+    <row r="547" ht="15.75" customHeight="1"/>
+    <row r="548" ht="15.75" customHeight="1"/>
+    <row r="549" ht="15.75" customHeight="1"/>
+    <row r="550" ht="15.75" customHeight="1"/>
+    <row r="551" ht="15.75" customHeight="1"/>
+    <row r="552" ht="15.75" customHeight="1"/>
+    <row r="553" ht="15.75" customHeight="1"/>
+    <row r="554" ht="15.75" customHeight="1"/>
+    <row r="555" ht="15.75" customHeight="1"/>
+    <row r="556" ht="15.75" customHeight="1"/>
+    <row r="557" ht="15.75" customHeight="1"/>
+    <row r="558" ht="15.75" customHeight="1"/>
+    <row r="559" ht="15.75" customHeight="1"/>
+    <row r="560" ht="15.75" customHeight="1"/>
+    <row r="561" ht="15.75" customHeight="1"/>
+    <row r="562" ht="15.75" customHeight="1"/>
+    <row r="563" ht="15.75" customHeight="1"/>
+    <row r="564" ht="15.75" customHeight="1"/>
+    <row r="565" ht="15.75" customHeight="1"/>
+    <row r="566" ht="15.75" customHeight="1"/>
+    <row r="567" ht="15.75" customHeight="1"/>
+    <row r="568" ht="15.75" customHeight="1"/>
+    <row r="569" ht="15.75" customHeight="1"/>
+    <row r="570" ht="15.75" customHeight="1"/>
+    <row r="571" ht="15.75" customHeight="1"/>
+    <row r="572" ht="15.75" customHeight="1"/>
+    <row r="573" ht="15.75" customHeight="1"/>
+    <row r="574" ht="15.75" customHeight="1"/>
+    <row r="575" ht="15.75" customHeight="1"/>
+    <row r="576" ht="15.75" customHeight="1"/>
+    <row r="577" ht="15.75" customHeight="1"/>
+    <row r="578" ht="15.75" customHeight="1"/>
+    <row r="579" ht="15.75" customHeight="1"/>
+    <row r="580" ht="15.75" customHeight="1"/>
+    <row r="581" ht="15.75" customHeight="1"/>
+    <row r="582" ht="15.75" customHeight="1"/>
+    <row r="583" ht="15.75" customHeight="1"/>
+    <row r="584" ht="15.75" customHeight="1"/>
+    <row r="585" ht="15.75" customHeight="1"/>
+    <row r="586" ht="15.75" customHeight="1"/>
+    <row r="587" ht="15.75" customHeight="1"/>
+    <row r="588" ht="15.75" customHeight="1"/>
+    <row r="589" ht="15.75" customHeight="1"/>
+    <row r="590" ht="15.75" customHeight="1"/>
+    <row r="591" ht="15.75" customHeight="1"/>
+    <row r="592" ht="15.75" customHeight="1"/>
+    <row r="593" ht="15.75" customHeight="1"/>
+    <row r="594" ht="15.75" customHeight="1"/>
+    <row r="595" ht="15.75" customHeight="1"/>
+    <row r="596" ht="15.75" customHeight="1"/>
+    <row r="597" ht="15.75" customHeight="1"/>
+    <row r="598" ht="15.75" customHeight="1"/>
+    <row r="599" ht="15.75" customHeight="1"/>
+    <row r="600" ht="15.75" customHeight="1"/>
+    <row r="601" ht="15.75" customHeight="1"/>
+    <row r="602" ht="15.75" customHeight="1"/>
+    <row r="603" ht="15.75" customHeight="1"/>
+    <row r="604" ht="15.75" customHeight="1"/>
+    <row r="605" ht="15.75" customHeight="1"/>
+    <row r="606" ht="15.75" customHeight="1"/>
+    <row r="607" ht="15.75" customHeight="1"/>
+    <row r="608" ht="15.75" customHeight="1"/>
+    <row r="609" ht="15.75" customHeight="1"/>
+    <row r="610" ht="15.75" customHeight="1"/>
+    <row r="611" ht="15.75" customHeight="1"/>
+    <row r="612" ht="15.75" customHeight="1"/>
+    <row r="613" ht="15.75" customHeight="1"/>
+    <row r="614" ht="15.75" customHeight="1"/>
+    <row r="615" ht="15.75" customHeight="1"/>
+    <row r="616" ht="15.75" customHeight="1"/>
+    <row r="617" ht="15.75" customHeight="1"/>
+    <row r="618" ht="15.75" customHeight="1"/>
+    <row r="619" ht="15.75" customHeight="1"/>
+    <row r="620" ht="15.75" customHeight="1"/>
+    <row r="621" ht="15.75" customHeight="1"/>
+    <row r="622" ht="15.75" customHeight="1"/>
+    <row r="623" ht="15.75" customHeight="1"/>
+    <row r="624" ht="15.75" customHeight="1"/>
+    <row r="625" ht="15.75" customHeight="1"/>
+    <row r="626" ht="15.75" customHeight="1"/>
+    <row r="627" ht="15.75" customHeight="1"/>
+    <row r="628" ht="15.75" customHeight="1"/>
+    <row r="629" ht="15.75" customHeight="1"/>
+    <row r="630" ht="15.75" customHeight="1"/>
+    <row r="631" ht="15.75" customHeight="1"/>
+    <row r="632" ht="15.75" customHeight="1"/>
+    <row r="633" ht="15.75" customHeight="1"/>
+    <row r="634" ht="15.75" customHeight="1"/>
+    <row r="635" ht="15.75" customHeight="1"/>
+    <row r="636" ht="15.75" customHeight="1"/>
+    <row r="637" ht="15.75" customHeight="1"/>
+    <row r="638" ht="15.75" customHeight="1"/>
+    <row r="639" ht="15.75" customHeight="1"/>
+    <row r="640" ht="15.75" customHeight="1"/>
+    <row r="641" ht="15.75" customHeight="1"/>
+    <row r="642" ht="15.75" customHeight="1"/>
+    <row r="643" ht="15.75" customHeight="1"/>
+    <row r="644" ht="15.75" customHeight="1"/>
+    <row r="645" ht="15.75" customHeight="1"/>
+    <row r="646" ht="15.75" customHeight="1"/>
+    <row r="647" ht="15.75" customHeight="1"/>
+    <row r="648" ht="15.75" customHeight="1"/>
+    <row r="649" ht="15.75" customHeight="1"/>
+    <row r="650" ht="15.75" customHeight="1"/>
+    <row r="651" ht="15.75" customHeight="1"/>
+    <row r="652" ht="15.75" customHeight="1"/>
+    <row r="653" ht="15.75" customHeight="1"/>
+    <row r="654" ht="15.75" customHeight="1"/>
+    <row r="655" ht="15.75" customHeight="1"/>
+    <row r="656" ht="15.75" customHeight="1"/>
+    <row r="657" ht="15.75" customHeight="1"/>
+    <row r="658" ht="15.75" customHeight="1"/>
+    <row r="659" ht="15.75" customHeight="1"/>
+    <row r="660" ht="15.75" customHeight="1"/>
+    <row r="661" ht="15.75" customHeight="1"/>
+    <row r="662" ht="15.75" customHeight="1"/>
+    <row r="663" ht="15.75" customHeight="1"/>
+    <row r="664" ht="15.75" customHeight="1"/>
+    <row r="665" ht="15.75" customHeight="1"/>
+    <row r="666" ht="15.75" customHeight="1"/>
+    <row r="667" ht="15.75" customHeight="1"/>
+    <row r="668" ht="15.75" customHeight="1"/>
+    <row r="669" ht="15.75" customHeight="1"/>
+    <row r="670" ht="15.75" customHeight="1"/>
+    <row r="671" ht="15.75" customHeight="1"/>
+    <row r="672" ht="15.75" customHeight="1"/>
+    <row r="673" ht="15.75" customHeight="1"/>
+    <row r="674" ht="15.75" customHeight="1"/>
+    <row r="675" ht="15.75" customHeight="1"/>
+    <row r="676" ht="15.75" customHeight="1"/>
+    <row r="677" ht="15.75" customHeight="1"/>
+    <row r="678" ht="15.75" customHeight="1"/>
+    <row r="679" ht="15.75" customHeight="1"/>
+    <row r="680" ht="15.75" customHeight="1"/>
+    <row r="681" ht="15.75" customHeight="1"/>
+    <row r="682" ht="15.75" customHeight="1"/>
+    <row r="683" ht="15.75" customHeight="1"/>
+    <row r="684" ht="15.75" customHeight="1"/>
+    <row r="685" ht="15.75" customHeight="1"/>
+    <row r="686" ht="15.75" customHeight="1"/>
+    <row r="687" ht="15.75" customHeight="1"/>
+    <row r="688" ht="15.75" customHeight="1"/>
+    <row r="689" ht="15.75" customHeight="1"/>
+    <row r="690" ht="15.75" customHeight="1"/>
+    <row r="691" ht="15.75" customHeight="1"/>
+    <row r="692" ht="15.75" customHeight="1"/>
+    <row r="693" ht="15.75" customHeight="1"/>
+    <row r="694" ht="15.75" customHeight="1"/>
+    <row r="695" ht="15.75" customHeight="1"/>
+    <row r="696" ht="15.75" customHeight="1"/>
+    <row r="697" ht="15.75" customHeight="1"/>
+    <row r="698" ht="15.75" customHeight="1"/>
+    <row r="699" ht="15.75" customHeight="1"/>
+    <row r="700" ht="15.75" customHeight="1"/>
+    <row r="701" ht="15.75" customHeight="1"/>
+    <row r="702" ht="15.75" customHeight="1"/>
+    <row r="703" ht="15.75" customHeight="1"/>
+    <row r="704" ht="15.75" customHeight="1"/>
+    <row r="705" ht="15.75" customHeight="1"/>
+    <row r="706" ht="15.75" customHeight="1"/>
+    <row r="707" ht="15.75" customHeight="1"/>
+    <row r="708" ht="15.75" customHeight="1"/>
+    <row r="709" ht="15.75" customHeight="1"/>
+    <row r="710" ht="15.75" customHeight="1"/>
+    <row r="711" ht="15.75" customHeight="1"/>
+    <row r="712" ht="15.75" customHeight="1"/>
+    <row r="713" ht="15.75" customHeight="1"/>
+    <row r="714" ht="15.75" customHeight="1"/>
+    <row r="715" ht="15.75" customHeight="1"/>
+    <row r="716" ht="15.75" customHeight="1"/>
+    <row r="717" ht="15.75" customHeight="1"/>
+    <row r="718" ht="15.75" customHeight="1"/>
+    <row r="719" ht="15.75" customHeight="1"/>
+    <row r="720" ht="15.75" customHeight="1"/>
+    <row r="721" ht="15.75" customHeight="1"/>
+    <row r="722" ht="15.75" customHeight="1"/>
+    <row r="723" ht="15.75" customHeight="1"/>
+    <row r="724" ht="15.75" customHeight="1"/>
+    <row r="725" ht="15.75" customHeight="1"/>
+    <row r="726" ht="15.75" customHeight="1"/>
+    <row r="727" ht="15.75" customHeight="1"/>
+    <row r="728" ht="15.75" customHeight="1"/>
+    <row r="729" ht="15.75" customHeight="1"/>
+    <row r="730" ht="15.75" customHeight="1"/>
+    <row r="731" ht="15.75" customHeight="1"/>
+    <row r="732" ht="15.75" customHeight="1"/>
+    <row r="733" ht="15.75" customHeight="1"/>
+    <row r="734" ht="15.75" customHeight="1"/>
+    <row r="735" ht="15.75" customHeight="1"/>
+    <row r="736" ht="15.75" customHeight="1"/>
+    <row r="737" ht="15.75" customHeight="1"/>
+    <row r="738" ht="15.75" customHeight="1"/>
+    <row r="739" ht="15.75" customHeight="1"/>
+    <row r="740" ht="15.75" customHeight="1"/>
+    <row r="741" ht="15.75" customHeight="1"/>
+    <row r="742" ht="15.75" customHeight="1"/>
+    <row r="743" ht="15.75" customHeight="1"/>
+    <row r="744" ht="15.75" customHeight="1"/>
+    <row r="745" ht="15.75" customHeight="1"/>
+    <row r="746" ht="15.75" customHeight="1"/>
+    <row r="747" ht="15.75" customHeight="1"/>
+    <row r="748" ht="15.75" customHeight="1"/>
+    <row r="749" ht="15.75" customHeight="1"/>
+    <row r="750" ht="15.75" customHeight="1"/>
+    <row r="751" ht="15.75" customHeight="1"/>
+    <row r="752" ht="15.75" customHeight="1"/>
+    <row r="753" ht="15.75" customHeight="1"/>
+    <row r="754" ht="15.75" customHeight="1"/>
+    <row r="755" ht="15.75" customHeight="1"/>
+    <row r="756" ht="15.75" customHeight="1"/>
+    <row r="757" ht="15.75" customHeight="1"/>
+    <row r="758" ht="15.75" customHeight="1"/>
+    <row r="759" ht="15.75" customHeight="1"/>
+    <row r="760" ht="15.75" customHeight="1"/>
+    <row r="761" ht="15.75" customHeight="1"/>
+    <row r="762" ht="15.75" customHeight="1"/>
+    <row r="763" ht="15.75" customHeight="1"/>
+    <row r="764" ht="15.75" customHeight="1"/>
+    <row r="765" ht="15.75" customHeight="1"/>
+    <row r="766" ht="15.75" customHeight="1"/>
+    <row r="767" ht="15.75" customHeight="1"/>
+    <row r="768" ht="15.75" customHeight="1"/>
+    <row r="769" ht="15.75" customHeight="1"/>
+    <row r="770" ht="15.75" customHeight="1"/>
+    <row r="771" ht="15.75" customHeight="1"/>
+    <row r="772" ht="15.75" customHeight="1"/>
+    <row r="773" ht="15.75" customHeight="1"/>
+    <row r="774" ht="15.75" customHeight="1"/>
+    <row r="775" ht="15.75" customHeight="1"/>
+    <row r="776" ht="15.75" customHeight="1"/>
+    <row r="777" ht="15.75" customHeight="1"/>
+    <row r="778" ht="15.75" customHeight="1"/>
+    <row r="779" ht="15.75" customHeight="1"/>
+    <row r="780" ht="15.75" customHeight="1"/>
+    <row r="781" ht="15.75" customHeight="1"/>
+    <row r="782" ht="15.75" customHeight="1"/>
+    <row r="783" ht="15.75" customHeight="1"/>
+    <row r="784" ht="15.75" customHeight="1"/>
+    <row r="785" ht="15.75" customHeight="1"/>
+    <row r="786" ht="15.75" customHeight="1"/>
+    <row r="787" ht="15.75" customHeight="1"/>
+    <row r="788" ht="15.75" customHeight="1"/>
+    <row r="789" ht="15.75" customHeight="1"/>
+    <row r="790" ht="15.75" customHeight="1"/>
+    <row r="791" ht="15.75" customHeight="1"/>
+    <row r="792" ht="15.75" customHeight="1"/>
+    <row r="793" ht="15.75" customHeight="1"/>
+    <row r="794" ht="15.75" customHeight="1"/>
+    <row r="795" ht="15.75" customHeight="1"/>
+    <row r="796" ht="15.75" customHeight="1"/>
+    <row r="797" ht="15.75" customHeight="1"/>
+    <row r="798" ht="15.75" customHeight="1"/>
+    <row r="799" ht="15.75" customHeight="1"/>
+    <row r="800" ht="15.75" customHeight="1"/>
+    <row r="801" ht="15.75" customHeight="1"/>
+    <row r="802" ht="15.75" customHeight="1"/>
+    <row r="803" ht="15.75" customHeight="1"/>
+    <row r="804" ht="15.75" customHeight="1"/>
+    <row r="805" ht="15.75" customHeight="1"/>
+    <row r="806" ht="15.75" customHeight="1"/>
+    <row r="807" ht="15.75" customHeight="1"/>
+    <row r="808" ht="15.75" customHeight="1"/>
+    <row r="809" ht="15.75" customHeight="1"/>
+    <row r="810" ht="15.75" customHeight="1"/>
+    <row r="811" ht="15.75" customHeight="1"/>
+    <row r="812" ht="15.75" customHeight="1"/>
+    <row r="813" ht="15.75" customHeight="1"/>
+    <row r="814" ht="15.75" customHeight="1"/>
+    <row r="815" ht="15.75" customHeight="1"/>
+    <row r="816" ht="15.75" customHeight="1"/>
+    <row r="817" ht="15.75" customHeight="1"/>
+    <row r="818" ht="15.75" customHeight="1"/>
+    <row r="819" ht="15.75" customHeight="1"/>
+    <row r="820" ht="15.75" customHeight="1"/>
+    <row r="821" ht="15.75" customHeight="1"/>
+    <row r="822" ht="15.75" customHeight="1"/>
+    <row r="823" ht="15.75" customHeight="1"/>
+    <row r="824" ht="15.75" customHeight="1"/>
+    <row r="825" ht="15.75" customHeight="1"/>
+    <row r="826" ht="15.75" customHeight="1"/>
+    <row r="827" ht="15.75" customHeight="1"/>
+    <row r="828" ht="15.75" customHeight="1"/>
+    <row r="829" ht="15.75" customHeight="1"/>
+    <row r="830" ht="15.75" customHeight="1"/>
+    <row r="831" ht="15.75" customHeight="1"/>
+    <row r="832" ht="15.75" customHeight="1"/>
+    <row r="833" ht="15.75" customHeight="1"/>
+    <row r="834" ht="15.75" customHeight="1"/>
+    <row r="835" ht="15.75" customHeight="1"/>
+    <row r="836" ht="15.75" customHeight="1"/>
+    <row r="837" ht="15.75" customHeight="1"/>
+    <row r="838" ht="15.75" customHeight="1"/>
+    <row r="839" ht="15.75" customHeight="1"/>
+    <row r="840" ht="15.75" customHeight="1"/>
+    <row r="841" ht="15.75" customHeight="1"/>
+    <row r="842" ht="15.75" customHeight="1"/>
+    <row r="843" ht="15.75" customHeight="1"/>
+    <row r="844" ht="15.75" customHeight="1"/>
+    <row r="845" ht="15.75" customHeight="1"/>
+    <row r="846" ht="15.75" customHeight="1"/>
+    <row r="847" ht="15.75" customHeight="1"/>
+    <row r="848" ht="15.75" customHeight="1"/>
+    <row r="849" ht="15.75" customHeight="1"/>
+    <row r="850" ht="15.75" customHeight="1"/>
+    <row r="851" ht="15.75" customHeight="1"/>
+    <row r="852" ht="15.75" customHeight="1"/>
+    <row r="853" ht="15.75" customHeight="1"/>
+    <row r="854" ht="15.75" customHeight="1"/>
+    <row r="855" ht="15.75" customHeight="1"/>
+    <row r="856" ht="15.75" customHeight="1"/>
+    <row r="857" ht="15.75" customHeight="1"/>
+    <row r="858" ht="15.75" customHeight="1"/>
+    <row r="859" ht="15.75" customHeight="1"/>
+    <row r="860" ht="15.75" customHeight="1"/>
+    <row r="861" ht="15.75" customHeight="1"/>
+    <row r="862" ht="15.75" customHeight="1"/>
+    <row r="863" ht="15.75" customHeight="1"/>
+    <row r="864" ht="15.75" customHeight="1"/>
+    <row r="865" ht="15.75" customHeight="1"/>
+    <row r="866" ht="15.75" customHeight="1"/>
+    <row r="867" ht="15.75" customHeight="1"/>
+    <row r="868" ht="15.75" customHeight="1"/>
+    <row r="869" ht="15.75" customHeight="1"/>
+    <row r="870" ht="15.75" customHeight="1"/>
+    <row r="871" ht="15.75" customHeight="1"/>
+    <row r="872" ht="15.75" customHeight="1"/>
+    <row r="873" ht="15.75" customHeight="1"/>
+    <row r="874" ht="15.75" customHeight="1"/>
+    <row r="875" ht="15.75" customHeight="1"/>
+    <row r="876" ht="15.75" customHeight="1"/>
+    <row r="877" ht="15.75" customHeight="1"/>
+    <row r="878" ht="15.75" customHeight="1"/>
+    <row r="879" ht="15.75" customHeight="1"/>
+    <row r="880" ht="15.75" customHeight="1"/>
+    <row r="881" ht="15.75" customHeight="1"/>
+    <row r="882" ht="15.75" customHeight="1"/>
+    <row r="883" ht="15.75" customHeight="1"/>
+    <row r="884" ht="15.75" customHeight="1"/>
+    <row r="885" ht="15.75" customHeight="1"/>
+    <row r="886" ht="15.75" customHeight="1"/>
+    <row r="887" ht="15.75" customHeight="1"/>
+    <row r="888" ht="15.75" customHeight="1"/>
+    <row r="889" ht="15.75" customHeight="1"/>
+    <row r="890" ht="15.75" customHeight="1"/>
+    <row r="891" ht="15.75" customHeight="1"/>
+    <row r="892" ht="15.75" customHeight="1"/>
+    <row r="893" ht="15.75" customHeight="1"/>
+    <row r="894" ht="15.75" customHeight="1"/>
+    <row r="895" ht="15.75" customHeight="1"/>
+    <row r="896" ht="15.75" customHeight="1"/>
+    <row r="897" ht="15.75" customHeight="1"/>
+    <row r="898" ht="15.75" customHeight="1"/>
+    <row r="899" ht="15.75" customHeight="1"/>
+    <row r="900" ht="15.75" customHeight="1"/>
+    <row r="901" ht="15.75" customHeight="1"/>
+    <row r="902" ht="15.75" customHeight="1"/>
+    <row r="903" ht="15.75" customHeight="1"/>
+    <row r="904" ht="15.75" customHeight="1"/>
+    <row r="905" ht="15.75" customHeight="1"/>
+    <row r="906" ht="15.75" customHeight="1"/>
+    <row r="907" ht="15.75" customHeight="1"/>
+    <row r="908" ht="15.75" customHeight="1"/>
+    <row r="909" ht="15.75" customHeight="1"/>
+    <row r="910" ht="15.75" customHeight="1"/>
+    <row r="911" ht="15.75" customHeight="1"/>
+    <row r="912" ht="15.75" customHeight="1"/>
+    <row r="913" ht="15.75" customHeight="1"/>
+    <row r="914" ht="15.75" customHeight="1"/>
+    <row r="915" ht="15.75" customHeight="1"/>
+    <row r="916" ht="15.75" customHeight="1"/>
+    <row r="917" ht="15.75" customHeight="1"/>
+    <row r="918" ht="15.75" customHeight="1"/>
+    <row r="919" ht="15.75" customHeight="1"/>
+    <row r="920" ht="15.75" customHeight="1"/>
+    <row r="921" ht="15.75" customHeight="1"/>
+    <row r="922" ht="15.75" customHeight="1"/>
+    <row r="923" ht="15.75" customHeight="1"/>
+    <row r="924" ht="15.75" customHeight="1"/>
+    <row r="925" ht="15.75" customHeight="1"/>
+    <row r="926" ht="15.75" customHeight="1"/>
+    <row r="927" ht="15.75" customHeight="1"/>
+    <row r="928" ht="15.75" customHeight="1"/>
+    <row r="929" ht="15.75" customHeight="1"/>
+    <row r="930" ht="15.75" customHeight="1"/>
+    <row r="931" ht="15.75" customHeight="1"/>
+    <row r="932" ht="15.75" customHeight="1"/>
+    <row r="933" ht="15.75" customHeight="1"/>
+    <row r="934" ht="15.75" customHeight="1"/>
+    <row r="935" ht="15.75" customHeight="1"/>
+    <row r="936" ht="15.75" customHeight="1"/>
+    <row r="937" ht="15.75" customHeight="1"/>
+    <row r="938" ht="15.75" customHeight="1"/>
+    <row r="939" ht="15.75" customHeight="1"/>
+    <row r="940" ht="15.75" customHeight="1"/>
+    <row r="941" ht="15.75" customHeight="1"/>
+    <row r="942" ht="15.75" customHeight="1"/>
+    <row r="943" ht="15.75" customHeight="1"/>
+    <row r="944" ht="15.75" customHeight="1"/>
+    <row r="945" ht="15.75" customHeight="1"/>
+    <row r="946" ht="15.75" customHeight="1"/>
+    <row r="947" ht="15.75" customHeight="1"/>
+    <row r="948" ht="15.75" customHeight="1"/>
+    <row r="949" ht="15.75" customHeight="1"/>
+    <row r="950" ht="15.75" customHeight="1"/>
+    <row r="951" ht="15.75" customHeight="1"/>
+    <row r="952" ht="15.75" customHeight="1"/>
+    <row r="953" ht="15.75" customHeight="1"/>
+    <row r="954" ht="15.75" customHeight="1"/>
+    <row r="955" ht="15.75" customHeight="1"/>
+    <row r="956" ht="15.75" customHeight="1"/>
+    <row r="957" ht="15.75" customHeight="1"/>
+    <row r="958" ht="15.75" customHeight="1"/>
+    <row r="959" ht="15.75" customHeight="1"/>
+    <row r="960" ht="15.75" customHeight="1"/>
+    <row r="961" ht="15.75" customHeight="1"/>
+    <row r="962" ht="15.75" customHeight="1"/>
+    <row r="963" ht="15.75" customHeight="1"/>
+    <row r="964" ht="15.75" customHeight="1"/>
+    <row r="965" ht="15.75" customHeight="1"/>
+    <row r="966" ht="15.75" customHeight="1"/>
+    <row r="967" ht="15.75" customHeight="1"/>
+    <row r="968" ht="15.75" customHeight="1"/>
+    <row r="969" ht="15.75" customHeight="1"/>
+    <row r="970" ht="15.75" customHeight="1"/>
+    <row r="971" ht="15.75" customHeight="1"/>
+    <row r="972" ht="15.75" customHeight="1"/>
+    <row r="973" ht="15.75" customHeight="1"/>
+    <row r="974" ht="15.75" customHeight="1"/>
+    <row r="975" ht="15.75" customHeight="1"/>
+    <row r="976" ht="15.75" customHeight="1"/>
+    <row r="977" ht="15.75" customHeight="1"/>
+    <row r="978" ht="15.75" customHeight="1"/>
+    <row r="979" ht="15.75" customHeight="1"/>
+    <row r="980" ht="15.75" customHeight="1"/>
+    <row r="981" ht="15.75" customHeight="1"/>
+    <row r="982" ht="15.75" customHeight="1"/>
+    <row r="983" ht="15.75" customHeight="1"/>
+    <row r="984" ht="15.75" customHeight="1"/>
+    <row r="985" ht="15.75" customHeight="1"/>
+    <row r="986" ht="15.75" customHeight="1"/>
+    <row r="987" ht="15.75" customHeight="1"/>
+    <row r="988" ht="15.75" customHeight="1"/>
+    <row r="989" ht="15.75" customHeight="1"/>
+    <row r="990" ht="15.75" customHeight="1"/>
+    <row r="991" ht="15.75" customHeight="1"/>
+    <row r="992" ht="15.75" customHeight="1"/>
+    <row r="993" ht="15.75" customHeight="1"/>
+    <row r="994" ht="15.75" customHeight="1"/>
+    <row r="995" ht="15.75" customHeight="1"/>
+    <row r="996" ht="15.75" customHeight="1"/>
+    <row r="997" ht="15.75" customHeight="1"/>
+    <row r="998" ht="15.75" customHeight="1"/>
+    <row r="999" ht="15.75" customHeight="1"/>
+    <row r="1000" ht="15.75" customHeight="1"/>
   </sheetData>
   <autoFilter ref="C1:C1000" xr:uid="{00000000-0001-0000-0000-000000000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:AL1000">

</xml_diff>